<commit_message>
Batch experiments and plots are pending; Experiments need to be rerun
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\postCompletion\research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\postCompletion\research\Accelerated-Blind-CNN-Descent-ABCD-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233A6EBE-D6A6-475A-AA12-BC8DF5E1B9AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC133DFF-0D37-4994-B182-D589B4A50C20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Experiment number</t>
   </si>
@@ -81,7 +81,10 @@
     <t>nine</t>
   </si>
   <si>
-    <t>Test Accuracy (%)</t>
+    <t>CIFAR-10 Test Accuracy (%)</t>
+  </si>
+  <si>
+    <t>MNIST Test Accuracy (%)</t>
   </si>
 </sst>
 </file>
@@ -408,20 +411,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -434,8 +438,11 @@
       <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -446,7 +453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -457,7 +464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -468,7 +475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -479,7 +486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -490,7 +497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -501,7 +508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -512,7 +519,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -523,7 +530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>

</xml_diff>